<commit_message>
Farben angespasst, Test für Urban-Burger :)
</commit_message>
<xml_diff>
--- a/data/Bern/Meta_Bern.xlsx
+++ b/data/Bern/Meta_Bern.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/Desktop/Work/Network/Bern/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mburger\Desktop\GitHub\Logger_Network\data\Bern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6BAC39-827B-6940-8D65-9771C66D7661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt 1 - metadata_gen_2" sheetId="1" r:id="rId1"/>
@@ -898,11 +897,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -981,7 +980,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1094,13 +1093,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1239,15 +1322,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -2371,37 +2490,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:XFD68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="21" style="1" customWidth="1"/>
-    <col min="12" max="12" width="27.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.83203125" style="1" customWidth="1"/>
-    <col min="16" max="17" width="5.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.33203125" style="1"/>
+    <col min="12" max="12" width="27.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.85546875" style="1" customWidth="1"/>
+    <col min="16" max="17" width="5.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2454,7 +2573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2503,7 +2622,7 @@
       </c>
       <c r="Q2" s="10"/>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="20.25" customHeight="1">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2552,56 +2671,56 @@
       </c>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="27">
+    <row r="4" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="18">
         <v>7</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="21">
         <v>46.944789999999998</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="21">
         <v>7.42713</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="22">
         <v>2599124.4</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="22">
         <v>1199300.1000000001</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="22">
         <v>528.6</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="32"/>
-    </row>
-    <row r="5" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O4" s="23"/>
+      <c r="P4" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="23"/>
+    </row>
+    <row r="5" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="18">
         <v>8</v>
       </c>
@@ -2650,7 +2769,7 @@
       </c>
       <c r="Q5" s="23"/>
     </row>
-    <row r="6" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="18">
         <v>9</v>
       </c>
@@ -2699,7 +2818,7 @@
       </c>
       <c r="Q6" s="23"/>
     </row>
-    <row r="7" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="18">
         <v>10</v>
       </c>
@@ -2748,7 +2867,7 @@
       </c>
       <c r="Q7" s="23"/>
     </row>
-    <row r="8" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="18">
         <v>13</v>
       </c>
@@ -2797,7 +2916,7 @@
       </c>
       <c r="Q8" s="23"/>
     </row>
-    <row r="9" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="18">
         <v>14</v>
       </c>
@@ -2846,7 +2965,7 @@
       </c>
       <c r="Q9" s="23"/>
     </row>
-    <row r="10" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="18">
         <v>16</v>
       </c>
@@ -2895,7 +3014,7 @@
       </c>
       <c r="Q10" s="23"/>
     </row>
-    <row r="11" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="18">
         <v>17</v>
       </c>
@@ -2944,7 +3063,7 @@
       </c>
       <c r="Q11" s="23"/>
     </row>
-    <row r="12" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="18">
         <v>19</v>
       </c>
@@ -2993,56 +3112,56 @@
       </c>
       <c r="Q12" s="23"/>
     </row>
-    <row r="13" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="27">
+    <row r="13" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="18">
         <v>21</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="21">
         <v>46.939639999999997</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="21">
         <v>7.4416599999999997</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="22">
         <v>2600230.5</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="22">
         <v>1198727.8999999999</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="22">
         <v>502.9</v>
       </c>
-      <c r="J13" s="29" t="s">
+      <c r="J13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="29" t="s">
+      <c r="N13" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="32"/>
-      <c r="P13" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="32"/>
-    </row>
-    <row r="14" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O13" s="23"/>
+      <c r="P13" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="23"/>
+    </row>
+    <row r="14" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="18">
         <v>22</v>
       </c>
@@ -3091,7 +3210,7 @@
       </c>
       <c r="Q14" s="23"/>
     </row>
-    <row r="15" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="18">
         <v>23</v>
       </c>
@@ -3140,7 +3259,7 @@
       </c>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="18">
         <v>25</v>
       </c>
@@ -3189,7 +3308,7 @@
       </c>
       <c r="Q16" s="23"/>
     </row>
-    <row r="17" spans="1:17" s="45" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" s="45" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="39">
         <v>26</v>
       </c>
@@ -3238,7 +3357,7 @@
       </c>
       <c r="Q17" s="44"/>
     </row>
-    <row r="18" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="18">
         <v>28</v>
       </c>
@@ -3287,7 +3406,7 @@
       </c>
       <c r="Q18" s="23"/>
     </row>
-    <row r="19" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="18">
         <v>30</v>
       </c>
@@ -3336,7 +3455,7 @@
       </c>
       <c r="Q19" s="23"/>
     </row>
-    <row r="20" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="18">
         <v>31</v>
       </c>
@@ -3385,7 +3504,7 @@
       </c>
       <c r="Q20" s="23"/>
     </row>
-    <row r="21" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="18">
         <v>32</v>
       </c>
@@ -3434,54 +3553,54 @@
       </c>
       <c r="Q21" s="23"/>
     </row>
-    <row r="22" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="27">
+    <row r="22" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="18">
         <v>33</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="21">
         <v>46.937980000000003</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="21">
         <v>7.4565599999999996</v>
       </c>
-      <c r="G22" s="31">
+      <c r="G22" s="22">
         <v>2601365.1</v>
       </c>
-      <c r="H22" s="31">
+      <c r="H22" s="22">
         <v>1198543.6000000001</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="22">
         <v>535.20000000000005</v>
       </c>
-      <c r="J22" s="29" t="s">
+      <c r="J22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="L22" s="29" t="s">
+      <c r="L22" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="M22" s="29" t="s">
+      <c r="M22" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="32"/>
-    </row>
-    <row r="23" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="23"/>
+    </row>
+    <row r="23" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="18">
         <v>34</v>
       </c>
@@ -3530,7 +3649,7 @@
       </c>
       <c r="Q23" s="23"/>
     </row>
-    <row r="24" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="18">
         <v>36</v>
       </c>
@@ -3579,7 +3698,7 @@
       </c>
       <c r="Q24" s="23"/>
     </row>
-    <row r="25" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="18">
         <v>37</v>
       </c>
@@ -3628,7 +3747,7 @@
       </c>
       <c r="Q25" s="23"/>
     </row>
-    <row r="26" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="18">
         <v>38</v>
       </c>
@@ -3677,7 +3796,7 @@
       </c>
       <c r="Q26" s="23"/>
     </row>
-    <row r="27" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="18">
         <v>39</v>
       </c>
@@ -3726,7 +3845,7 @@
       </c>
       <c r="Q27" s="23"/>
     </row>
-    <row r="28" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="18">
         <v>41</v>
       </c>
@@ -3775,7 +3894,7 @@
       </c>
       <c r="Q28" s="23"/>
     </row>
-    <row r="29" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="18">
         <v>42</v>
       </c>
@@ -3824,7 +3943,7 @@
       </c>
       <c r="Q29" s="23"/>
     </row>
-    <row r="30" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="18">
         <v>45</v>
       </c>
@@ -3873,7 +3992,7 @@
       </c>
       <c r="Q30" s="23"/>
     </row>
-    <row r="31" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="18">
         <v>48</v>
       </c>
@@ -3922,7 +4041,7 @@
       </c>
       <c r="Q31" s="23"/>
     </row>
-    <row r="32" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="18">
         <v>51</v>
       </c>
@@ -3971,7 +4090,7 @@
       </c>
       <c r="Q32" s="23"/>
     </row>
-    <row r="33" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="18">
         <v>52</v>
       </c>
@@ -4020,7 +4139,7 @@
       </c>
       <c r="Q33" s="23"/>
     </row>
-    <row r="34" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="18">
         <v>53</v>
       </c>
@@ -4069,7 +4188,7 @@
       </c>
       <c r="Q34" s="23"/>
     </row>
-    <row r="35" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="18">
         <v>55</v>
       </c>
@@ -4118,7 +4237,7 @@
       </c>
       <c r="Q35" s="23"/>
     </row>
-    <row r="36" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="18">
         <v>57</v>
       </c>
@@ -4167,7 +4286,7 @@
       </c>
       <c r="Q36" s="23"/>
     </row>
-    <row r="37" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="18">
         <v>58</v>
       </c>
@@ -4216,7 +4335,7 @@
       </c>
       <c r="Q37" s="23"/>
     </row>
-    <row r="38" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="18">
         <v>59</v>
       </c>
@@ -4265,7 +4384,7 @@
       </c>
       <c r="Q38" s="23"/>
     </row>
-    <row r="39" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="18">
         <v>61</v>
       </c>
@@ -4314,7 +4433,7 @@
       </c>
       <c r="Q39" s="23"/>
     </row>
-    <row r="40" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="18">
         <v>62</v>
       </c>
@@ -4363,7 +4482,7 @@
       </c>
       <c r="Q40" s="23"/>
     </row>
-    <row r="41" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="18">
         <v>65</v>
       </c>
@@ -4412,7 +4531,7 @@
       </c>
       <c r="Q41" s="23"/>
     </row>
-    <row r="42" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="18">
         <v>69</v>
       </c>
@@ -4461,7 +4580,7 @@
       </c>
       <c r="Q42" s="23"/>
     </row>
-    <row r="43" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="18">
         <v>70</v>
       </c>
@@ -4510,7 +4629,7 @@
       </c>
       <c r="Q43" s="23"/>
     </row>
-    <row r="44" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="18">
         <v>71</v>
       </c>
@@ -4559,7 +4678,7 @@
       </c>
       <c r="Q44" s="23"/>
     </row>
-    <row r="45" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="18">
         <v>73</v>
       </c>
@@ -4608,7 +4727,7 @@
       </c>
       <c r="Q45" s="23"/>
     </row>
-    <row r="46" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="18">
         <v>76</v>
       </c>
@@ -4657,7 +4776,7 @@
       </c>
       <c r="Q46" s="23"/>
     </row>
-    <row r="47" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="18">
         <v>78</v>
       </c>
@@ -4706,7 +4825,7 @@
       </c>
       <c r="Q47" s="23"/>
     </row>
-    <row r="48" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="18">
         <v>79</v>
       </c>
@@ -4755,7 +4874,7 @@
       </c>
       <c r="Q48" s="23"/>
     </row>
-    <row r="49" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="18">
         <v>80</v>
       </c>
@@ -4804,7 +4923,7 @@
       </c>
       <c r="Q49" s="23"/>
     </row>
-    <row r="50" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="18">
         <v>82</v>
       </c>
@@ -4853,7 +4972,7 @@
       </c>
       <c r="Q50" s="23"/>
     </row>
-    <row r="51" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="18">
         <v>83</v>
       </c>
@@ -4902,7 +5021,7 @@
       </c>
       <c r="Q51" s="23"/>
     </row>
-    <row r="52" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="18">
         <v>86</v>
       </c>
@@ -4951,7 +5070,7 @@
       </c>
       <c r="Q52" s="23"/>
     </row>
-    <row r="53" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="18">
         <v>87</v>
       </c>
@@ -5000,7 +5119,7 @@
       </c>
       <c r="Q53" s="23"/>
     </row>
-    <row r="54" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:17" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="27">
         <v>89</v>
       </c>
@@ -5049,7 +5168,7 @@
       </c>
       <c r="Q54" s="32"/>
     </row>
-    <row r="55" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="18">
         <v>98</v>
       </c>
@@ -5098,7 +5217,7 @@
       </c>
       <c r="Q55" s="23"/>
     </row>
-    <row r="56" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="18">
         <v>99</v>
       </c>
@@ -5147,7 +5266,7 @@
       </c>
       <c r="Q56" s="23"/>
     </row>
-    <row r="57" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="18">
         <v>101</v>
       </c>
@@ -5196,7 +5315,7 @@
       </c>
       <c r="Q57" s="23"/>
     </row>
-    <row r="58" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="18">
         <v>102</v>
       </c>
@@ -5245,7 +5364,7 @@
       </c>
       <c r="Q58" s="23"/>
     </row>
-    <row r="59" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="18">
         <v>111</v>
       </c>
@@ -5294,7 +5413,7 @@
       </c>
       <c r="Q59" s="23"/>
     </row>
-    <row r="60" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="18">
         <v>112</v>
       </c>
@@ -5343,7 +5462,7 @@
       </c>
       <c r="Q60" s="23"/>
     </row>
-    <row r="61" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="18">
         <v>113</v>
       </c>
@@ -5392,7 +5511,7 @@
       </c>
       <c r="Q61" s="23"/>
     </row>
-    <row r="62" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="18">
         <v>116</v>
       </c>
@@ -5441,7 +5560,7 @@
       </c>
       <c r="Q62" s="23"/>
     </row>
-    <row r="63" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="18">
         <v>117</v>
       </c>
@@ -5490,7 +5609,7 @@
       </c>
       <c r="Q63" s="23"/>
     </row>
-    <row r="64" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="18">
         <v>124</v>
       </c>
@@ -5539,7 +5658,7 @@
       </c>
       <c r="Q64" s="23"/>
     </row>
-    <row r="65" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="18">
         <v>126</v>
       </c>
@@ -5588,7 +5707,7 @@
       </c>
       <c r="Q65" s="23"/>
     </row>
-    <row r="66" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="18">
         <v>127</v>
       </c>
@@ -5637,7 +5756,7 @@
       </c>
       <c r="Q66" s="23"/>
     </row>
-    <row r="67" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A67" s="18">
         <v>128</v>
       </c>
@@ -5654,10 +5773,10 @@
       <c r="F67" s="21">
         <v>7.47159</v>
       </c>
-      <c r="G67" s="46">
+      <c r="G67" s="58">
         <v>2602508.69</v>
       </c>
-      <c r="H67" s="47">
+      <c r="H67" s="59">
         <v>1200259.1299999999</v>
       </c>
       <c r="I67" s="22">
@@ -5674,56 +5793,56 @@
       <c r="P67" s="21"/>
       <c r="Q67" s="23"/>
     </row>
-    <row r="68" spans="1:17" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="27">
+    <row r="68" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A68" s="18">
         <v>129</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="D68" s="29" t="s">
+      <c r="D68" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="E68" s="30">
+      <c r="E68" s="21">
         <v>46.947339999999997</v>
       </c>
-      <c r="F68" s="30">
+      <c r="F68" s="21">
         <v>7.4363900000000003</v>
       </c>
-      <c r="G68" s="30">
+      <c r="G68" s="21">
         <v>2599829</v>
       </c>
-      <c r="H68" s="31">
+      <c r="H68" s="22">
         <v>1199583.8</v>
       </c>
-      <c r="I68" s="31">
+      <c r="I68" s="22">
         <v>540.6</v>
       </c>
-      <c r="J68" s="29" t="s">
+      <c r="J68" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="K68" s="29" t="s">
+      <c r="K68" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="L68" s="29" t="s">
+      <c r="L68" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="M68" s="29" t="s">
+      <c r="M68" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N68" s="29" t="s">
+      <c r="N68" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="O68" s="32"/>
-      <c r="P68" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="32"/>
-    </row>
-    <row r="69" spans="1:17" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O68" s="23"/>
+      <c r="P68" s="21">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="23"/>
+    </row>
+    <row r="69" spans="1:17" s="25" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="18">
         <v>134</v>
       </c>
@@ -5766,7 +5885,7 @@
       </c>
       <c r="Q69" s="23"/>
     </row>
-    <row r="70" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="18">
         <v>135</v>
       </c>
@@ -5815,7 +5934,7 @@
       </c>
       <c r="Q70" s="23"/>
     </row>
-    <row r="71" spans="1:17" s="45" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:17" s="45" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A71" s="39">
         <v>136</v>
       </c>
@@ -5864,7 +5983,7 @@
       </c>
       <c r="Q71" s="44"/>
     </row>
-    <row r="72" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="18">
         <v>141</v>
       </c>
@@ -5913,7 +6032,7 @@
       </c>
       <c r="Q72" s="23"/>
     </row>
-    <row r="73" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A73" s="18">
         <v>142</v>
       </c>
@@ -5962,7 +6081,7 @@
       </c>
       <c r="Q73" s="23"/>
     </row>
-    <row r="74" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A74" s="18">
         <v>143</v>
       </c>
@@ -6011,105 +6130,105 @@
       </c>
       <c r="Q74" s="23"/>
     </row>
-    <row r="75" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="18">
+    <row r="75" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A75" s="52">
         <v>144</v>
       </c>
-      <c r="B75" s="19" t="s">
+      <c r="B75" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D75" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="E75" s="21">
+      <c r="E75" s="55">
         <v>46.961779999999997</v>
       </c>
-      <c r="F75" s="21">
+      <c r="F75" s="55">
         <v>7.4348099999999997</v>
       </c>
-      <c r="G75" s="22">
+      <c r="G75" s="56">
         <v>2599709.2999999998</v>
       </c>
-      <c r="H75" s="22">
+      <c r="H75" s="56">
         <v>1201189.5</v>
       </c>
-      <c r="I75" s="22">
+      <c r="I75" s="56">
         <v>573.6</v>
       </c>
-      <c r="J75" s="20" t="s">
+      <c r="J75" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="K75" s="20" t="s">
+      <c r="K75" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="L75" s="20" t="s">
+      <c r="L75" s="54" t="s">
         <v>240</v>
       </c>
-      <c r="M75" s="20" t="s">
+      <c r="M75" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="N75" s="20" t="s">
+      <c r="N75" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="O75" s="23"/>
-      <c r="P75" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q75" s="23"/>
-    </row>
-    <row r="76" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="18">
+      <c r="O75" s="57"/>
+      <c r="P75" s="55">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="57"/>
+    </row>
+    <row r="76" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A76" s="46">
         <v>152</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B76" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="E76" s="21">
+      <c r="E76" s="49">
         <v>46.958129999999997</v>
       </c>
-      <c r="F76" s="21">
+      <c r="F76" s="49">
         <v>7.4880699999999996</v>
       </c>
-      <c r="G76" s="21">
+      <c r="G76" s="49">
         <v>2603763</v>
       </c>
-      <c r="H76" s="22">
+      <c r="H76" s="50">
         <v>1200784.8</v>
       </c>
-      <c r="I76" s="21">
+      <c r="I76" s="49">
         <v>552</v>
       </c>
-      <c r="J76" s="20" t="s">
+      <c r="J76" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="K76" s="20" t="s">
+      <c r="K76" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="L76" s="20" t="s">
+      <c r="L76" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="M76" s="20" t="s">
+      <c r="M76" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="N76" s="20" t="s">
+      <c r="N76" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="O76" s="23"/>
-      <c r="P76" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q76" s="23"/>
-    </row>
-    <row r="77" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O76" s="51"/>
+      <c r="P76" s="49">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="51"/>
+    </row>
+    <row r="77" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A77" s="18">
         <v>153</v>
       </c>
@@ -6158,7 +6277,7 @@
       </c>
       <c r="Q77" s="23"/>
     </row>
-    <row r="78" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A78" s="18">
         <v>154</v>
       </c>
@@ -6207,7 +6326,7 @@
       </c>
       <c r="Q78" s="23"/>
     </row>
-    <row r="79" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A79" s="18">
         <v>155</v>
       </c>
@@ -6256,7 +6375,7 @@
       </c>
       <c r="Q79" s="23"/>
     </row>
-    <row r="80" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A80" s="18">
         <v>156</v>
       </c>
@@ -6305,7 +6424,7 @@
       </c>
       <c r="Q80" s="23"/>
     </row>
-    <row r="81" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A81" s="18">
         <v>161</v>
       </c>
@@ -6354,7 +6473,7 @@
       </c>
       <c r="Q81" s="23"/>
     </row>
-    <row r="82" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A82" s="18">
         <v>162</v>
       </c>
@@ -6403,7 +6522,7 @@
       </c>
       <c r="Q82" s="23"/>
     </row>
-    <row r="83" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A83" s="26" t="s">
         <v>278</v>
       </c>
@@ -6452,7 +6571,7 @@
       </c>
       <c r="Q83" s="23"/>
     </row>
-    <row r="84" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A84" s="26" t="s">
         <v>286</v>
       </c>
@@ -6501,7 +6620,7 @@
       </c>
       <c r="Q84" s="23"/>
     </row>
-    <row r="85" spans="1:17" s="11" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:17" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A85" s="26" t="s">
         <v>287</v>
       </c>
@@ -6551,7 +6670,7 @@
       <c r="Q85" s="23"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q101">
+  <sortState ref="A2:Q101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>